<commit_message>
[UPDATE] Source & Data
</commit_message>
<xml_diff>
--- a/data/Radiomics_changed.xlsx
+++ b/data/Radiomics_changed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Git\sa-uta8-utaut\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E2746D-CE7E-4225-8C74-78189E2D2827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D478CCB-B219-4F3F-9FC4-166516D991EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1306,11 +1306,20 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1320,15 +1329,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1934,7 +1934,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X14" sqref="X14"/>
+      <selection pane="bottomLeft" activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1945,32 +1945,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
+      <c r="A1" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="H1" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>182</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>9</v>
@@ -68879,7 +68879,7 @@
       <c r="E2" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="119"/>
+      <c r="F2" s="114"/>
       <c r="G2" s="115" t="s">
         <v>89</v>
       </c>
@@ -68894,7 +68894,7 @@
       <c r="E3" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="119"/>
+      <c r="F3" s="114"/>
       <c r="G3" s="115"/>
     </row>
     <row r="4" spans="1:7">
@@ -68907,7 +68907,7 @@
       <c r="E4" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="120"/>
+      <c r="F4" s="116"/>
       <c r="G4" s="115" t="s">
         <v>93</v>
       </c>
@@ -68922,7 +68922,7 @@
       <c r="E5" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="120"/>
+      <c r="F5" s="116"/>
       <c r="G5" s="115"/>
     </row>
     <row r="6" spans="1:7">
@@ -68933,7 +68933,7 @@
         <v>95</v>
       </c>
       <c r="E6" s="24"/>
-      <c r="F6" s="121"/>
+      <c r="F6" s="117"/>
       <c r="G6" s="115" t="s">
         <v>96</v>
       </c>
@@ -68946,7 +68946,7 @@
         <v>97</v>
       </c>
       <c r="E7" s="24"/>
-      <c r="F7" s="121"/>
+      <c r="F7" s="117"/>
       <c r="G7" s="115"/>
     </row>
     <row r="8" spans="1:7">
@@ -68957,7 +68957,7 @@
         <v>98</v>
       </c>
       <c r="E8" s="24"/>
-      <c r="F8" s="116"/>
+      <c r="F8" s="119"/>
       <c r="G8" s="115" t="s">
         <v>99</v>
       </c>
@@ -68973,7 +68973,7 @@
         <v>101</v>
       </c>
       <c r="E9" s="24"/>
-      <c r="F9" s="116"/>
+      <c r="F9" s="119"/>
       <c r="G9" s="115"/>
     </row>
     <row r="10" spans="1:7">
@@ -68992,7 +68992,7 @@
       <c r="E10" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="117"/>
+      <c r="F10" s="120"/>
       <c r="G10" s="115" t="s">
         <v>104</v>
       </c>
@@ -69013,7 +69013,7 @@
       <c r="E11" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="117"/>
+      <c r="F11" s="120"/>
       <c r="G11" s="115"/>
     </row>
     <row r="12" spans="1:7">
@@ -69032,7 +69032,7 @@
       <c r="E12" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="118"/>
+      <c r="F12" s="121"/>
       <c r="G12" s="115" t="s">
         <v>107</v>
       </c>
@@ -69053,7 +69053,7 @@
       <c r="E13" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="118"/>
+      <c r="F13" s="121"/>
       <c r="G13" s="115"/>
     </row>
     <row r="14" spans="1:7">
@@ -69072,7 +69072,7 @@
       <c r="E14" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="114"/>
+      <c r="F14" s="118"/>
       <c r="G14" s="115" t="s">
         <v>111</v>
       </c>
@@ -69093,7 +69093,7 @@
       <c r="E15" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="114"/>
+      <c r="F15" s="118"/>
       <c r="G15" s="115"/>
     </row>
     <row r="16" spans="1:7">
@@ -69516,12 +69516,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="F8:F9"/>
@@ -69530,6 +69524,12 @@
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="G12:G13"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>